<commit_message>
Latest version after break
</commit_message>
<xml_diff>
--- a/Testing/Test_Files/extra_information.xlsx
+++ b/Testing/Test_Files/extra_information.xlsx
@@ -82,6 +82,39 @@
     <t xml:space="preserve">00002881</t>
   </si>
   <si>
+    <t xml:space="preserve">T_dicoccum_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emmu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00002882</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emmer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T_dicoccum_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00002883</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T_dicoccum_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00002884</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T_dicoccum_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00002885</t>
+  </si>
+  <si>
     <t xml:space="preserve">T_monococcum_3</t>
   </si>
   <si>
@@ -97,6 +130,51 @@
     <t xml:space="preserve">00002887</t>
   </si>
   <si>
+    <t xml:space="preserve">T_ispahanicum_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00002889</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T_ispahanicum_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00002894</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T_dicoccum_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00002897</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bottom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00002898</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T_dicoccum_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00002902</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00002903</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T_ispahanicum_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00002910</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00002912</t>
+  </si>
+  <si>
     <t xml:space="preserve">T_monococcum_5</t>
   </si>
   <si>
@@ -227,84 +305,6 @@
   </si>
   <si>
     <t xml:space="preserve">00003905</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T_dicoccum_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emmu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00002882</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emmer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T_dicoccum_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00002883</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T_dicoccum_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00002884</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T_dicoccum_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00002885</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T_dicoccum_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">top</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00002897</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bottom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00002898</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T_dicoccum_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00002902</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00002903</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T_ispahanicum_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00002889</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T_ispahanicum_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00002894</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T_ispahanicum_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00002910</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00002912</t>
   </si>
 </sst>
 </file>
@@ -440,13 +440,15 @@
   </sheetPr>
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O30" activeCellId="0" sqref="O30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E:E"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.68"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -561,7 +563,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>798</v>
+        <v>869</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>22</v>
@@ -573,13 +575,13 @@
         <v>14</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>17</v>
@@ -587,7 +589,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>21</v>
@@ -596,25 +598,25 @@
         <v>12</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>793</v>
+        <v>854</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>68.8</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>68.8</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>17</v>
@@ -622,19 +624,19 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>1212</v>
+        <v>1101</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>68.8</v>
@@ -643,13 +645,13 @@
         <v>14</v>
       </c>
       <c r="H6" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>17</v>
@@ -657,19 +659,19 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>1218</v>
+        <v>822</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>68.8</v>
@@ -678,13 +680,13 @@
         <v>14</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>17</v>
@@ -692,19 +694,19 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>1068</v>
+        <v>798</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>68.8</v>
@@ -727,19 +729,19 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="C9" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>1162</v>
+        <v>793</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>68.8</v>
@@ -762,19 +764,17 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>26</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>1186</v>
+        <v>1224</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>68.8</v>
@@ -783,13 +783,13 @@
         <v>14</v>
       </c>
       <c r="H10" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>17</v>
@@ -797,19 +797,17 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>1036</v>
+        <v>1279</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>68.8</v>
@@ -818,13 +816,13 @@
         <v>14</v>
       </c>
       <c r="H11" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>17</v>
@@ -832,19 +830,17 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>1086</v>
+        <v>511</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F12" s="1" t="n">
         <v>68.8</v>
@@ -853,13 +849,13 @@
         <v>14</v>
       </c>
       <c r="H12" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>17</v>
@@ -867,19 +863,17 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>1224</v>
+        <v>658</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F13" s="1" t="n">
         <v>68.8</v>
@@ -888,13 +882,13 @@
         <v>14</v>
       </c>
       <c r="H13" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>17</v>
@@ -902,19 +896,17 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>1285</v>
+        <v>476</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F14" s="1" t="n">
         <v>68.8</v>
@@ -923,13 +915,13 @@
         <v>14</v>
       </c>
       <c r="H14" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>17</v>
@@ -939,17 +931,15 @@
       <c r="A15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>1288</v>
+        <v>740</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F15" s="1" t="n">
         <v>68.8</v>
@@ -958,13 +948,13 @@
         <v>14</v>
       </c>
       <c r="H15" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>17</v>
@@ -972,16 +962,14 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>1238</v>
+        <v>666</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>49</v>
@@ -993,13 +981,13 @@
         <v>14</v>
       </c>
       <c r="H16" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>17</v>
@@ -1007,20 +995,18 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>816</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="1" t="n">
-        <v>1400</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="F17" s="1" t="n">
         <v>68.8</v>
       </c>
@@ -1028,13 +1014,13 @@
         <v>14</v>
       </c>
       <c r="H17" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>17</v>
@@ -1042,16 +1028,16 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="C18" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>1200</v>
+        <v>1212</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>53</v>
@@ -1080,13 +1066,13 @@
         <v>54</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>1285</v>
+        <v>1218</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>55</v>
@@ -1115,13 +1101,13 @@
         <v>56</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>1367</v>
+        <v>1068</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>57</v>
@@ -1150,16 +1136,16 @@
         <v>58</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>1162</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="1" t="n">
-        <v>807</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>60</v>
       </c>
       <c r="F21" s="1" t="n">
         <v>68.8</v>
@@ -1182,19 +1168,19 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>1186</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="1" t="n">
-        <v>916</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>62</v>
       </c>
       <c r="F22" s="1" t="n">
         <v>68.8</v>
@@ -1217,18 +1203,18 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="C23" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>831</v>
-      </c>
-      <c r="E23" s="6" t="s">
+        <v>1036</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>64</v>
       </c>
       <c r="F23" s="1" t="n">
@@ -1255,15 +1241,15 @@
         <v>65</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>881</v>
-      </c>
-      <c r="E24" s="6" t="s">
+        <v>1086</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>66</v>
       </c>
       <c r="F24" s="1" t="n">
@@ -1290,15 +1276,15 @@
         <v>67</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>845</v>
-      </c>
-      <c r="E25" s="6" t="s">
+        <v>1224</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>68</v>
       </c>
       <c r="F25" s="1" t="n">
@@ -1325,17 +1311,17 @@
         <v>69</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>1285</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="1" t="n">
-        <v>869</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="F26" s="1" t="n">
         <v>68.8</v>
       </c>
@@ -1343,13 +1329,13 @@
         <v>14</v>
       </c>
       <c r="H26" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>17</v>
@@ -1357,19 +1343,19 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="1" t="n">
-        <v>854</v>
+        <v>1288</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F27" s="1" t="n">
         <v>68.8</v>
@@ -1378,13 +1364,13 @@
         <v>14</v>
       </c>
       <c r="H27" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>17</v>
@@ -1392,19 +1378,19 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>1101</v>
+        <v>1238</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F28" s="1" t="n">
         <v>68.8</v>
@@ -1413,13 +1399,13 @@
         <v>14</v>
       </c>
       <c r="H28" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="K28" s="3" t="s">
         <v>17</v>
@@ -1427,19 +1413,19 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>822</v>
+        <v>1400</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F29" s="1" t="n">
         <v>68.8</v>
@@ -1448,13 +1434,13 @@
         <v>14</v>
       </c>
       <c r="H29" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="K29" s="3" t="s">
         <v>17</v>
@@ -1462,17 +1448,19 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B30" s="1"/>
+        <v>78</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="C30" s="4" t="s">
-        <v>81</v>
+        <v>12</v>
       </c>
       <c r="D30" s="1" t="n">
-        <v>511</v>
+        <v>1200</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F30" s="1" t="n">
         <v>68.8</v>
@@ -1481,13 +1469,13 @@
         <v>14</v>
       </c>
       <c r="H30" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="K30" s="3" t="s">
         <v>17</v>
@@ -1497,15 +1485,17 @@
       <c r="A31" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B31" s="1"/>
+      <c r="B31" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="C31" s="4" t="s">
-        <v>83</v>
+        <v>12</v>
       </c>
       <c r="D31" s="1" t="n">
-        <v>658</v>
+        <v>1285</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F31" s="1" t="n">
         <v>68.8</v>
@@ -1514,13 +1504,13 @@
         <v>14</v>
       </c>
       <c r="H31" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="K31" s="3" t="s">
         <v>17</v>
@@ -1528,17 +1518,19 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B32" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="C32" s="4" t="s">
-        <v>81</v>
+        <v>12</v>
       </c>
       <c r="D32" s="1" t="n">
-        <v>476</v>
+        <v>1367</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F32" s="1" t="n">
         <v>68.8</v>
@@ -1547,13 +1539,13 @@
         <v>14</v>
       </c>
       <c r="H32" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="K32" s="3" t="s">
         <v>17</v>
@@ -1561,17 +1553,19 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B33" s="1"/>
       <c r="C33" s="4" t="s">
-        <v>83</v>
+        <v>12</v>
       </c>
       <c r="D33" s="1" t="n">
-        <v>740</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>87</v>
+        <v>807</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="F33" s="1" t="n">
         <v>68.8</v>
@@ -1580,13 +1574,13 @@
         <v>14</v>
       </c>
       <c r="H33" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="K33" s="3" t="s">
         <v>17</v>
@@ -1594,18 +1588,20 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>916</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D34" s="1" t="n">
-        <v>1224</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>89</v>
-      </c>
       <c r="F34" s="1" t="n">
         <v>68.8</v>
       </c>
@@ -1613,13 +1609,13 @@
         <v>14</v>
       </c>
       <c r="H34" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="K34" s="3" t="s">
         <v>17</v>
@@ -1627,18 +1623,20 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>831</v>
+      </c>
+      <c r="E35" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="1" t="n">
-        <v>1279</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>91</v>
-      </c>
       <c r="F35" s="1" t="n">
         <v>68.8</v>
       </c>
@@ -1646,13 +1644,13 @@
         <v>14</v>
       </c>
       <c r="H35" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="K35" s="3" t="s">
         <v>17</v>
@@ -1660,18 +1658,20 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <v>881</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D36" s="1" t="n">
-        <v>666</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>93</v>
-      </c>
       <c r="F36" s="1" t="n">
         <v>68.8</v>
       </c>
@@ -1679,13 +1679,13 @@
         <v>14</v>
       </c>
       <c r="H36" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="K36" s="3" t="s">
         <v>17</v>
@@ -1693,16 +1693,18 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B37" s="1"/>
+        <v>93</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="C37" s="4" t="s">
-        <v>83</v>
+        <v>12</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>816</v>
-      </c>
-      <c r="E37" s="5" t="s">
+        <v>845</v>
+      </c>
+      <c r="E37" s="6" t="s">
         <v>94</v>
       </c>
       <c r="F37" s="1" t="n">
@@ -1712,13 +1714,13 @@
         <v>14</v>
       </c>
       <c r="H37" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="K37" s="3" t="s">
         <v>17</v>

</xml_diff>